<commit_message>
changes in spec file
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Riomed\Cellma4Automation\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60F59B1-D598-4842-B50B-C800D6EEF7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF83B7A-36F6-4CD6-BB19-020F362008DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="21" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="219">
   <si>
     <t>username</t>
   </si>
@@ -603,9 +603,6 @@
   </si>
   <si>
     <t>Repair of rectum</t>
-  </si>
-  <si>
-    <t>Recommendation</t>
   </si>
   <si>
     <t>Edited Recommendation for testing</t>
@@ -1146,7 +1143,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1173,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>180</v>
@@ -1201,7 +1198,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1228,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>180</v>
@@ -1243,7 +1240,7 @@
         <v>177</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1255,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EDCE76-70F4-4473-B92F-8913C9A903B8}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,7 +1275,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>180</v>
@@ -1550,7 +1547,7 @@
         <v>153</v>
       </c>
       <c r="M1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1588,7 +1585,7 @@
         <v>154</v>
       </c>
       <c r="M2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1893,16 +1890,16 @@
     </row>
     <row r="2" spans="1:48" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>53</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>54</v>
@@ -2011,13 +2008,13 @@
         <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" t="s">
         <v>140</v>
       </c>
       <c r="E1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F1" t="s">
         <v>134</v>
@@ -2025,10 +2022,10 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" t="s">
         <v>183</v>
-      </c>
-      <c r="B2" t="s">
-        <v>184</v>
       </c>
       <c r="C2" t="s">
         <v>139</v>
@@ -2040,7 +2037,7 @@
         <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2074,13 +2071,13 @@
         <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" t="s">
         <v>140</v>
       </c>
       <c r="E1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F1" t="s">
         <v>134</v>
@@ -2088,10 +2085,10 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" t="s">
         <v>183</v>
-      </c>
-      <c r="B2" t="s">
-        <v>184</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -2100,10 +2097,10 @@
         <v>45453</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2139,10 +2136,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" t="s">
         <v>183</v>
-      </c>
-      <c r="B2" t="s">
-        <v>184</v>
       </c>
       <c r="C2" t="s">
         <v>131</v>
@@ -2182,30 +2179,30 @@
         <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D1" t="s">
         <v>140</v>
       </c>
       <c r="E1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F1" t="s">
         <v>134</v>
       </c>
       <c r="G1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>174</v>
@@ -2215,16 +2212,16 @@
         <v>45474</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I2" s="8"/>
     </row>
@@ -2237,7 +2234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE09E9A-9C0C-49EF-BEE4-12AF4C853339}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -2261,30 +2258,30 @@
         <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D1" t="s">
         <v>140</v>
       </c>
       <c r="E1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F1" t="s">
         <v>134</v>
       </c>
       <c r="G1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>174</v>
@@ -2294,16 +2291,16 @@
         <v>45474</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="F2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>219</v>
-      </c>
       <c r="H2" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2339,10 +2336,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>131</v>
@@ -2451,7 +2448,7 @@
         <v>103</v>
       </c>
       <c r="P1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q1" t="s">
         <v>89</v>
@@ -2496,7 +2493,7 @@
         <v>134</v>
       </c>
       <c r="AE1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -2525,13 +2522,13 @@
         <v>109</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" t="s">
         <v>194</v>
-      </c>
-      <c r="K2" t="s">
-        <v>195</v>
       </c>
       <c r="N2" t="s">
         <v>88</v>
@@ -2540,7 +2537,7 @@
         <v>104</v>
       </c>
       <c r="P2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q2" t="s">
         <v>90</v>
@@ -2567,7 +2564,7 @@
         <v>111</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Z2" t="s">
         <v>115</v>
@@ -2582,10 +2579,10 @@
         <v>117</v>
       </c>
       <c r="AD2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AE2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2710,16 +2707,16 @@
         <v>78</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>119</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>201</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>202</v>
       </c>
       <c r="K2" t="s">
         <v>94</v>
@@ -2731,7 +2728,7 @@
         <v>93</v>
       </c>
       <c r="P2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q2" t="s">
         <v>98</v>
@@ -2740,13 +2737,13 @@
         <v>119</v>
       </c>
       <c r="S2" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="T2" t="s">
+        <v>203</v>
+      </c>
+      <c r="U2" t="s">
         <v>205</v>
-      </c>
-      <c r="T2" t="s">
-        <v>204</v>
-      </c>
-      <c r="U2" t="s">
-        <v>206</v>
       </c>
       <c r="V2" t="s">
         <v>104</v>

</xml_diff>